<commit_message>
Remake source data files to fix 3A, add plates elsewhere
</commit_message>
<xml_diff>
--- a/source_data_files/Extended_Data_Figure_2_SourceData.xlsx
+++ b/source_data_files/Extended_Data_Figure_2_SourceData.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -455,6 +455,11 @@
           <t>Plating density</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Plates</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -475,6 +480,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>['BR00116991', 'BR00116992', 'BR00116993', 'BR00116994', 'BR00117015', 'BR00117016', 'BR00117017', 'BR00117019']</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -495,6 +505,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>['BR00116991', 'BR00116992', 'BR00116993', 'BR00116994', 'BR00117020', 'BR00117021']</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -515,6 +530,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>['BR00116991', 'BR00116992', 'BR00116993', 'BR00116994', 'BR00118050', 'BR00117006']</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -535,6 +555,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>['BR00117015', 'BR00117016', 'BR00117017', 'BR00117019', 'BR00117020', 'BR00117021']</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -555,6 +580,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>['BR00117015', 'BR00117016', 'BR00117017', 'BR00117019', 'BR00118050', 'BR00117006']</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -575,6 +605,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>['BR00116991', 'BR00116992', 'BR00116993', 'BR00116994', 'BR00118041', 'BR00118042', 'BR00118043', 'BR00118044']</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -595,6 +630,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>['BR00116991', 'BR00116992', 'BR00116993', 'BR00116994', 'BR00117000', 'BR00117003', 'BR00117004', 'BR00117005']</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -615,6 +655,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>['BR00117015', 'BR00117016', 'BR00117017', 'BR00117019', 'BR00118041', 'BR00118042', 'BR00118043', 'BR00118044']</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -635,6 +680,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>['BR00117015', 'BR00117016', 'BR00117017', 'BR00117019', 'BR00117000', 'BR00117003', 'BR00117004', 'BR00117005']</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -655,6 +705,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>['BR00117020', 'BR00117021', 'BR00118050', 'BR00117006']</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -675,6 +730,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>['BR00117020', 'BR00117021', 'BR00118041', 'BR00118042', 'BR00118043', 'BR00118044']</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -695,6 +755,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>['BR00117020', 'BR00117021', 'BR00117000', 'BR00117003', 'BR00117004', 'BR00117005']</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -715,6 +780,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>['BR00118050', 'BR00117006', 'BR00118041', 'BR00118042', 'BR00118043', 'BR00118044']</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -735,6 +805,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>['BR00118050', 'BR00117006', 'BR00117000', 'BR00117003', 'BR00117004', 'BR00117005']</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -755,6 +830,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>['BR00118041', 'BR00118042', 'BR00118043', 'BR00118044', 'BR00117000', 'BR00117003', 'BR00117004', 'BR00117005']</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -775,6 +855,11 @@
           <t>A549 - A549 80%</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>['BR00116991', 'BR00116992', 'BR00116993', 'BR00116994', 'BR00117008', 'BR00117009']</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -795,6 +880,11 @@
           <t>A549 - A549 80%</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>['BR00117015', 'BR00117016', 'BR00117017', 'BR00117019', 'BR00117008', 'BR00117009']</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -815,6 +905,11 @@
           <t>A549 - A549 80%</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>['BR00117020', 'BR00117021', 'BR00117008', 'BR00117009']</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -835,6 +930,11 @@
           <t>A549 - A549 80%</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>['BR00118050', 'BR00117006', 'BR00117008', 'BR00117009']</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -855,6 +955,11 @@
           <t>A549 - A549 80%</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>['BR00118041', 'BR00118042', 'BR00118043', 'BR00118044', 'BR00117008', 'BR00117009']</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -875,6 +980,11 @@
           <t>A549 - A549 80%</t>
         </is>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>['BR00117000', 'BR00117003', 'BR00117004', 'BR00117005', 'BR00117008', 'BR00117009']</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -895,6 +1005,11 @@
           <t>A549 - A549 120%</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>['BR00116991', 'BR00116992', 'BR00116993', 'BR00116994', 'BR00117054', 'BR00117055']</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -915,6 +1030,11 @@
           <t>A549 - A549 120%</t>
         </is>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>['BR00117015', 'BR00117016', 'BR00117017', 'BR00117019', 'BR00117054', 'BR00117055']</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -935,6 +1055,11 @@
           <t>A549 - A549 120%</t>
         </is>
       </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>['BR00117020', 'BR00117021', 'BR00117054', 'BR00117055']</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -955,6 +1080,11 @@
           <t>A549 - A549 120%</t>
         </is>
       </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>['BR00118050', 'BR00117006', 'BR00117054', 'BR00117055']</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -975,6 +1105,11 @@
           <t>A549 - A549 120%</t>
         </is>
       </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>['BR00118041', 'BR00118042', 'BR00118043', 'BR00118044', 'BR00117054', 'BR00117055']</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -995,6 +1130,11 @@
           <t>A549 - A549 120%</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>['BR00117000', 'BR00117003', 'BR00117004', 'BR00117005', 'BR00117054', 'BR00117055']</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -1013,6 +1153,11 @@
       <c r="D29" t="inlineStr">
         <is>
           <t>A549 80% - A549 120%</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>['BR00117008', 'BR00117009', 'BR00117054', 'BR00117055']</t>
         </is>
       </c>
     </row>
@@ -1027,7 +1172,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1056,6 +1201,11 @@
           <t>Matching between parental and Cas9</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Plates</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -1076,6 +1226,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>['BR00116991', 'BR00116992', 'BR00116993', 'BR00116994', 'BR00117015', 'BR00117016', 'BR00117017', 'BR00117019']</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -1096,6 +1251,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>['BR00116991', 'BR00116992', 'BR00116993', 'BR00116994', 'BR00117020', 'BR00117021']</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -1116,6 +1276,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>['BR00116991', 'BR00116992', 'BR00116993', 'BR00116994', 'BR00118050', 'BR00117006']</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -1136,6 +1301,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>['BR00117015', 'BR00117016', 'BR00117017', 'BR00117019', 'BR00117020', 'BR00117021']</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -1156,6 +1326,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>['BR00117015', 'BR00117016', 'BR00117017', 'BR00117019', 'BR00118050', 'BR00117006']</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -1176,6 +1351,11 @@
           <t>A549 - A549</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>['BR00117020', 'BR00117021', 'BR00118050', 'BR00117006']</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1196,6 +1376,11 @@
           <t>A549 - A549-Cas9</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>['BR00116991', 'BR00116992', 'BR00116993', 'BR00116994', 'BR00117050', 'BR00117051', 'BR00117052', 'BR00117053']</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1216,6 +1401,11 @@
           <t>A549 - A549-Cas9</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>['BR00117015', 'BR00117016', 'BR00117017', 'BR00117019', 'BR00117050', 'BR00117051', 'BR00117052', 'BR00117053']</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1236,6 +1426,11 @@
           <t>A549 - A549-Cas9</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>['BR00116991', 'BR00116992', 'BR00116993', 'BR00116994', 'BR00118041', 'BR00118042', 'BR00118043', 'BR00118044']</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1256,6 +1451,11 @@
           <t>A549 - A549-Cas9</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>['BR00116991', 'BR00116992', 'BR00116993', 'BR00116994', 'BR00117000', 'BR00117003', 'BR00117004', 'BR00117005']</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1276,6 +1476,11 @@
           <t>A549 - A549-Cas9</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>['BR00117015', 'BR00117016', 'BR00117017', 'BR00117019', 'BR00118041', 'BR00118042', 'BR00118043', 'BR00118044']</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1296,6 +1501,11 @@
           <t>A549 - A549-Cas9</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>['BR00117015', 'BR00117016', 'BR00117017', 'BR00117019', 'BR00117000', 'BR00117003', 'BR00117004', 'BR00117005']</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1316,6 +1526,11 @@
           <t>A549 - A549-Cas9</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>['BR00117020', 'BR00117021', 'BR00117050', 'BR00117051', 'BR00117052', 'BR00117053']</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1336,6 +1551,11 @@
           <t>A549 - A549-Cas9</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>['BR00118050', 'BR00117006', 'BR00117050', 'BR00117051', 'BR00117052', 'BR00117053']</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1356,6 +1576,11 @@
           <t>A549 - A549-Cas9</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>['BR00117020', 'BR00117021', 'BR00118041', 'BR00118042', 'BR00118043', 'BR00118044']</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1376,6 +1601,11 @@
           <t>A549 - A549-Cas9</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>['BR00117020', 'BR00117021', 'BR00117000', 'BR00117003', 'BR00117004', 'BR00117005']</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1396,6 +1626,11 @@
           <t>A549 - A549-Cas9</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>['BR00118050', 'BR00117006', 'BR00118041', 'BR00118042', 'BR00118043', 'BR00118044']</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1416,6 +1651,11 @@
           <t>A549 - A549-Cas9</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>['BR00118050', 'BR00117006', 'BR00117000', 'BR00117003', 'BR00117004', 'BR00117005']</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1436,6 +1676,11 @@
           <t>A549-Cas9 - A549-Cas9</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>['BR00117050', 'BR00117051', 'BR00117052', 'BR00117053', 'BR00118041', 'BR00118042', 'BR00118043', 'BR00118044']</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1456,6 +1701,11 @@
           <t>A549-Cas9 - A549-Cas9</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>['BR00117050', 'BR00117051', 'BR00117052', 'BR00117053', 'BR00117000', 'BR00117003', 'BR00117004', 'BR00117005']</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1474,6 +1724,11 @@
       <c r="D22" t="inlineStr">
         <is>
           <t>A549-Cas9 - A549-Cas9</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>['BR00118041', 'BR00118042', 'BR00118043', 'BR00118044', 'BR00117000', 'BR00117003', 'BR00117004', 'BR00117005']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
remake source data files after adding new sub panel
</commit_message>
<xml_diff>
--- a/source_data_files/Extended_Data_Figure_2_SourceData.xlsx
+++ b/source_data_files/Extended_Data_Figure_2_SourceData.xlsx
@@ -7,8 +7,8 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ED2A" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ED2B" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ED2B" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="ED2C" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>

<commit_message>
fix parentheses, rerun files/figures
</commit_message>
<xml_diff>
--- a/source_data_files/Extended_Data_Figure_2_SourceData.xlsx
+++ b/source_data_files/Extended_Data_Figure_2_SourceData.xlsx
@@ -786,7 +786,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>48.00668896321071</v>
+        <v>49.33110367892976</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -811,7 +811,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>7.545751633986928</v>
+        <v>10.45751633986928</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -836,7 +836,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>9.169934640522875</v>
+        <v>11.11111111111111</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -861,7 +861,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7.879084967320261</v>
+        <v>11.43790849673203</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -886,7 +886,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>9.490196078431373</v>
+        <v>10.7843137254902</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -911,7 +911,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6.403780068728522</v>
+        <v>10.99656357388316</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
@@ -936,7 +936,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7.243986254295532</v>
+        <v>9.965635738831615</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -961,7 +961,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>10.51890034364261</v>
+        <v>14.26116838487972</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -986,7 +986,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9.304123711340209</v>
+        <v>11.85567010309278</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1036,7 +1036,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>7.550819672131148</v>
+        <v>8.524590163934427</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>8.872131147540983</v>
+        <v>10.81967213114754</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1086,7 +1086,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>9.203278688524589</v>
+        <v>11.47540983606557</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1111,7 +1111,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>10.18688524590164</v>
+        <v>12.45901639344262</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1136,7 +1136,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>27.41176470588236</v>
+        <v>29.07563025210084</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1161,7 +1161,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>45.83277591973244</v>
+        <v>47.1571906354515</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>47.83612040133779</v>
+        <v>48.82943143812709</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1211,7 +1211,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>9.852941176470589</v>
+        <v>14.70588235294118</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1236,7 +1236,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>10.14705882352941</v>
+        <v>11.76470588235294</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1261,7 +1261,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>8.115120274914089</v>
+        <v>12.02749140893471</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1286,7 +1286,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>7.769759450171821</v>
+        <v>11.51202749140894</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1311,7 +1311,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>44.49163879598662</v>
+        <v>45.48494983277592</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1336,7 +1336,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>49.01003344481605</v>
+        <v>50.33444816053512</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1361,7 +1361,7 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>6.918300653594772</v>
+        <v>12.41830065359477</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -1386,7 +1386,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>10.47385620915033</v>
+        <v>12.09150326797386</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -1411,7 +1411,7 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>8.288659793814432</v>
+        <v>12.37113402061856</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -1436,7 +1436,7 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>7.243986254295532</v>
+        <v>9.965635738831615</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -1461,7 +1461,7 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>48.50501672240803</v>
+        <v>49.49832775919732</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -1532,7 +1532,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>48.00668896321071</v>
+        <v>49.33110367892976</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -1557,7 +1557,7 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>7.545751633986928</v>
+        <v>10.45751633986928</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -1582,7 +1582,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>9.173202614379084</v>
+        <v>11.43790849673203</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7.879084967320261</v>
+        <v>11.43790849673203</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -1632,7 +1632,7 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>9.490196078431373</v>
+        <v>10.7843137254902</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
@@ -1682,7 +1682,7 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>43.32107023411371</v>
+        <v>44.31438127090301</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
@@ -1707,7 +1707,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>45.32775919732441</v>
+        <v>46.32107023411371</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -1732,7 +1732,7 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>6.403780068728522</v>
+        <v>10.99656357388316</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -1757,7 +1757,7 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>7.243986254295532</v>
+        <v>9.965635738831615</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -1782,7 +1782,7 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>10.51890034364261</v>
+        <v>14.26116838487972</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1807,7 +1807,7 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>8.960481099656358</v>
+        <v>11.51202749140894</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1832,7 +1832,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>9.516339869281046</v>
+        <v>13.39869281045752</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1857,7 +1857,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>11.13398692810458</v>
+        <v>13.39869281045752</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1882,7 +1882,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>7.222950819672132</v>
+        <v>8.196721311475411</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>8.865573770491803</v>
+        <v>10.16393442622951</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1932,7 +1932,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>9.531147540983604</v>
+        <v>11.80327868852459</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1957,7 +1957,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>8.547540983606556</v>
+        <v>10.81967213114754</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1982,7 +1982,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>9.5</v>
+        <v>14.43298969072165</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -2007,7 +2007,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>8.634020618556701</v>
+        <v>12.88659793814433</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -2032,7 +2032,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>27.74789915966386</v>
+        <v>29.41176470588236</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>

</xml_diff>